<commit_message>
Se modifico redaccion de algunos docuemntos.
</commit_message>
<xml_diff>
--- a/02.Implementación de proyecto/Primer Sprint/SGySHT_ControlRiesgos_v1.xlsx
+++ b/02.Implementación de proyecto/Primer Sprint/SGySHT_ControlRiesgos_v1.xlsx
@@ -217,10 +217,10 @@
     <t>Los integrantes del equipo de desarrollo no administran de manera correcta el sofware de gestion de proyecto</t>
   </si>
   <si>
-    <t>Cambiar de software para llevar la gestion de seguimineto del proyecto</t>
-  </si>
-  <si>
-    <t>utilizar el software de gestion para administrar el proyecto a diario</t>
+    <t>utilizar y actualizar el software de gestion para administrar el proyecto a diario</t>
+  </si>
+  <si>
+    <t>Cambiar de software para llevar la gestion del seguimiento del proyecto</t>
   </si>
 </sst>
 </file>
@@ -891,7 +891,7 @@
   <dimension ref="A4:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="J20" sqref="A20:J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1253,10 +1253,10 @@
         <v>16</v>
       </c>
       <c r="F20" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="G20" s="20" t="s">
         <v>58</v>
-      </c>
-      <c r="G20" s="20" t="s">
-        <v>57</v>
       </c>
       <c r="H20" s="6">
         <v>43589</v>

</xml_diff>